<commit_message>
DB schema excel is updated
</commit_message>
<xml_diff>
--- a/DB_schema_broker_retailer.xlsx
+++ b/DB_schema_broker_retailer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pragalya Kanakaraj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00E29FF9-6360-4073-A10A-1D3FCDB9BCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03704173-9B1C-4A27-8725-137441B1F996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{893E6BC4-BA8D-4CB6-8A87-F5D96D0468C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{893E6BC4-BA8D-4CB6-8A87-F5D96D0468C5}"/>
   </bookViews>
   <sheets>
     <sheet name="static_Tables" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="256">
   <si>
     <t xml:space="preserve"> bid</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>b_established_year</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> b_shop_name</t>
   </si>
   <si>
     <t>b_person_name</t>
@@ -273,9 +270,6 @@
     <t>master_mandi_table</t>
   </si>
   <si>
-    <t>mandi_id</t>
-  </si>
-  <si>
     <t>mandi_location</t>
   </si>
   <si>
@@ -310,18 +304,6 @@
   </si>
   <si>
     <t>image_path</t>
-  </si>
-  <si>
-    <t>regional_name1</t>
-  </si>
-  <si>
-    <t>regional_name2</t>
-  </si>
-  <si>
-    <t>regional_name3</t>
-  </si>
-  <si>
-    <t>regional_name4</t>
   </si>
   <si>
     <t>bigint</t>
@@ -887,6 +869,60 @@
   </si>
   <si>
     <t>INSERT ,UPDATE , SELECT</t>
+  </si>
+  <si>
+    <t>business_branch_table</t>
+  </si>
+  <si>
+    <t>b_branch_id</t>
+  </si>
+  <si>
+    <t>b_shop_name</t>
+  </si>
+  <si>
+    <t>business_category_table</t>
+  </si>
+  <si>
+    <t>b_category_id</t>
+  </si>
+  <si>
+    <t>b_category_name</t>
+  </si>
+  <si>
+    <t>master_city</t>
+  </si>
+  <si>
+    <t>abbreviation</t>
+  </si>
+  <si>
+    <t>city_name</t>
+  </si>
+  <si>
+    <t>character varying(5)</t>
+  </si>
+  <si>
+    <t>city_abbreviation</t>
+  </si>
+  <si>
+    <t>b_privilege_user</t>
+  </si>
+  <si>
+    <t>mandi_abbrevation</t>
+  </si>
+  <si>
+    <t>product_regional_name</t>
+  </si>
+  <si>
+    <t>product_regional_id</t>
+  </si>
+  <si>
+    <t>category_regional_name</t>
+  </si>
+  <si>
+    <t>category_regional_id</t>
+  </si>
+  <si>
+    <t>category_id</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1043,14 +1079,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1365,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E971A767-F42F-4D75-9124-AF5DA9117968}">
-  <dimension ref="A1:B220"/>
+  <dimension ref="A1:B251"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1380,7 +1420,7 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1388,1133 +1428,1316 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
+      <c r="A6" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A12" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>242</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>124</v>
+      <c r="A14" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>124</v>
+      <c r="A18" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>24</v>
+      <c r="A19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="9"/>
+      <c r="A23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>21</v>
+      <c r="A25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="9"/>
+      <c r="A29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>38</v>
+        <v>249</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>30</v>
+      <c r="A32" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>125</v>
+      <c r="A33" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="A35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="B39" s="9"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="9"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="9"/>
+      <c r="A48" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B57" s="9"/>
+      <c r="A53" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="A58" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="9"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" s="9"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B71" s="9"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B76" s="9"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B79" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="3" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B69" s="9"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B75" s="9"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B81" s="9"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B82" s="3"/>
+      <c r="B82" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B86" s="3" t="s">
+      <c r="A84" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="A88" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B88" s="9"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B93" s="9"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>87</v>
+      <c r="A89" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="A95" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B95" s="9"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="2" t="s">
-        <v>47</v>
+      <c r="A96" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
-        <v>82</v>
+        <v>248</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>88</v>
+      <c r="A99" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="A100" s="13"/>
+      <c r="B100" s="13"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="A101" s="13"/>
+      <c r="B101" s="13"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>89</v>
+      <c r="A102" s="13"/>
+      <c r="B102" s="13"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B104" s="9"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B106" s="9"/>
+      <c r="A106" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A107" s="13"/>
+      <c r="B107" s="13"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A108" s="13"/>
+      <c r="B108" s="13"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A110" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B110" s="9"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="A111" s="2"/>
+      <c r="B111" s="3"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
-        <v>96</v>
+        <v>250</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B120" s="9"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B122" s="3" t="s">
+      <c r="A116" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B117" s="3" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A123" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B123" s="9"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>89</v>
+      <c r="A125" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B129" s="9"/>
+      <c r="A129" s="2"/>
+      <c r="B129" s="3"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A130" s="2"/>
+      <c r="B130" s="3"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B131" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="A131" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B131" s="9"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B132" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B136" s="9"/>
+      <c r="A132" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="A137" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B137" s="9"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B138" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B141" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B139" s="5" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="B142" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B143" s="9"/>
+      <c r="A143" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B146" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B150" s="9"/>
+      <c r="A146" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A151" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B151" s="9"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" s="2" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="B152" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B154" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A153" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B153" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B157" s="9"/>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A158" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>24</v>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="A160" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B160" s="9"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
-        <v>121</v>
+        <v>43</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>19</v>
+      <c r="A162" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A163" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A164" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A166" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>89</v>
+      <c r="A163" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A167" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>124</v>
-      </c>
+      <c r="A167" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B167" s="9"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A168" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B168" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A172" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
-        <v>126</v>
-      </c>
-      <c r="B173" t="s">
-        <v>24</v>
+      <c r="A168" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A169" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A170" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A174" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="A174" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B174" s="9"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" s="2" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A177" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A178" s="2" t="s">
+      <c r="A177" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B178" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A180" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>42</v>
+      <c r="B177" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A181" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B181" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A185" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B185" s="9"/>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A186" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A187" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B187" s="5" t="s">
-        <v>19</v>
+      <c r="A181" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B181" s="9"/>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A182" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A184" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A188" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B188" s="9"/>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A190" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A191" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B191" s="9"/>
+      <c r="A191" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" s="2" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A193" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B193" s="5" t="s">
-        <v>19</v>
+      <c r="A193" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A194" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A195" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A196" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A197" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B197" s="9"/>
+      <c r="A197" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" s="4" t="s">
-        <v>130</v>
+        <v>35</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A203" s="8"/>
-      <c r="B203" s="9"/>
+      <c r="A203" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A204" s="10"/>
-      <c r="B204" s="3"/>
+      <c r="A204" t="s">
+        <v>120</v>
+      </c>
+      <c r="B204" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A205" s="2"/>
-      <c r="B205" s="3"/>
+      <c r="A205" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A206" s="2"/>
-      <c r="B206" s="3"/>
+      <c r="A206" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A207" s="2"/>
-      <c r="B207" s="3"/>
+      <c r="A207" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A208" s="2"/>
-      <c r="B208" s="3"/>
+      <c r="A208" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A209" s="2"/>
-      <c r="B209" s="3"/>
+      <c r="A209" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A210" s="2"/>
-      <c r="B210" s="3"/>
+      <c r="A210" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A211" s="2"/>
-      <c r="B211" s="3"/>
+      <c r="A211" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A212" s="2"/>
-      <c r="B212" s="3"/>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A213" s="2"/>
-      <c r="B213" s="3"/>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A214" s="2"/>
-      <c r="B214" s="3"/>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A215" s="2"/>
-      <c r="B215" s="3"/>
+      <c r="A212" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A216" s="2"/>
-      <c r="B216" s="3"/>
+      <c r="A216" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B216" s="9"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A217" s="2"/>
-      <c r="B217" s="3"/>
+      <c r="A217" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A218" s="2"/>
-      <c r="B218" s="3"/>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A219" s="12"/>
-      <c r="B219" s="3"/>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A220" s="4"/>
-      <c r="B220" s="5"/>
+      <c r="A218" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A222" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B222" s="9"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A223" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A228" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B228" s="9"/>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A229" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B229" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A230" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B230" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A234" s="8"/>
+      <c r="B234" s="9"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A235" s="2"/>
+      <c r="B235" s="3"/>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A236" s="2"/>
+      <c r="B236" s="3"/>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A237" s="2"/>
+      <c r="B237" s="3"/>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238" s="2"/>
+      <c r="B238" s="3"/>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" s="2"/>
+      <c r="B239" s="3"/>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A240" s="2"/>
+      <c r="B240" s="3"/>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" s="2"/>
+      <c r="B241" s="3"/>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A242" s="2"/>
+      <c r="B242" s="3"/>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A243" s="2"/>
+      <c r="B243" s="3"/>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A244" s="2"/>
+      <c r="B244" s="3"/>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A245" s="2"/>
+      <c r="B245" s="3"/>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A246" s="2"/>
+      <c r="B246" s="3"/>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A247" s="2"/>
+      <c r="B247" s="3"/>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A248" s="2"/>
+      <c r="B248" s="3"/>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" s="2"/>
+      <c r="B249" s="3"/>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" s="11"/>
+      <c r="B250" s="3"/>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251" s="4"/>
+      <c r="B251" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2538,136 +2761,136 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
-        <v>132</v>
+      <c r="A2" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
-        <v>147</v>
+      <c r="A17" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -2676,72 +2899,72 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>156</v>
+        <v>147</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -2750,178 +2973,178 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B35" s="9"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B51" s="9"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B57" s="3"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="12" t="s">
-        <v>36</v>
+      <c r="A58" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="B58" s="3"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -2930,426 +3153,426 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B64" s="9"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="8" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B85" s="9"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="8" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B96" s="9"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B114" s="9"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3362,7 +3585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37B55EB4-751E-4260-AC38-F3846301219E}">
   <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
@@ -3375,712 +3598,712 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C10" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C11" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C12" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C16" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B17" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C17" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B18" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C19" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C24" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C25" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C26" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C27" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C31" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C32" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C33" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C34" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C38" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C39" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C40" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
+        <v>222</v>
+      </c>
+      <c r="C41" t="s">
         <v>228</v>
-      </c>
-      <c r="C41" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C45" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C46" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C47" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C48" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B52" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C52" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C53" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C54" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C55" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C59" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C60" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C61" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C62" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B66" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C66" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C67" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C68" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C69" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B73" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C73" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C74" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C75" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C76" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B80" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C80" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B81" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C81" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B82" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C82" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>226</v>
+      </c>
+      <c r="B83" t="s">
+        <v>222</v>
+      </c>
+      <c r="C83" t="s">
         <v>232</v>
-      </c>
-      <c r="B83" t="s">
-        <v>228</v>
-      </c>
-      <c r="C83" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B88" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C88" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C89" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C90" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C91" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B95" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C95" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C96" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C97" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C98" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B102" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C102" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C103" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C104" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C105" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B109" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C109" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C110" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C111" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C112" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B116" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C116" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C117" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C118" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C119" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B123" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C123" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B124" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B125" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B126" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B130" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C130" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C131" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C132" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C133" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel with cart,wishlist updated
</commit_message>
<xml_diff>
--- a/DB_schema_broker_retailer.xlsx
+++ b/DB_schema_broker_retailer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pragalya Kanakaraj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3D5B922-EE25-4B12-B93A-DE993B3EB400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97044E07-F1B5-4CC5-A81C-D66B41CA707B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{893E6BC4-BA8D-4CB6-8A87-F5D96D0468C5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="329">
   <si>
     <t xml:space="preserve"> bid</t>
   </si>
@@ -1078,12 +1078,85 @@
   <si>
     <t>Updates total_amount in order_table based on sum all items for that has same order_id</t>
   </si>
+  <si>
+    <t>cart_table</t>
+  </si>
+  <si>
+    <t>cart_id</t>
+  </si>
+  <si>
+    <t>cart_status</t>
+  </si>
+  <si>
+    <t>added_at</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INTEGER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(0 = In Cart, 1 = Moved to Wishlist, 2 = Removed)</t>
+    </r>
+  </si>
+  <si>
+    <t>whishlist_table</t>
+  </si>
+  <si>
+    <t>wishlist_id</t>
+  </si>
+  <si>
+    <t>wishlist_status</t>
+  </si>
+  <si>
+    <t>original_price</t>
+  </si>
+  <si>
+    <t>Price when added to wishlist</t>
+  </si>
+  <si>
+    <t>current_price</t>
+  </si>
+  <si>
+    <t>source_url</t>
+  </si>
+  <si>
+    <t>device_type</t>
+  </si>
+  <si>
+    <t>ip_address</t>
+  </si>
+  <si>
+    <t>character varying(45)</t>
+  </si>
+  <si>
+    <t>character varying(512)</t>
+  </si>
+  <si>
+    <t>price_drop_notification_sent</t>
+  </si>
+  <si>
+    <t>BOOLEAN DEFAULT FALSE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1135,6 +1208,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1144,7 +1238,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1214,11 +1308,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1243,6 +1363,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1559,7 +1684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E971A767-F42F-4D75-9124-AF5DA9117968}">
   <dimension ref="A1:C268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
       <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
@@ -2950,7 +3075,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3044,10 +3169,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB499724-65CB-4F13-8120-13A79F1C18BE}">
-  <dimension ref="A1:B146"/>
+  <dimension ref="A1:C184"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="K101" sqref="K101"/>
+    <sheetView topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3978,6 +4103,261 @@
       </c>
       <c r="B146" s="5" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B150" s="9"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="B160" s="17" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A163" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="B168" s="16"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C171" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A177" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A178" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A179" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A180" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="B180" s="17" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A181" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A182" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A184" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>